<commit_message>
Ajout de la licence, modification du fichier Data&Values.xlsx (description des feuilles du classeur
</commit_message>
<xml_diff>
--- a/InputsData/Data&Values.xlsx
+++ b/InputsData/Data&Values.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\grangeont\OneDrive - BRGM\Pro\AMORAD\ArticleCarteNationale\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\grangeont\OneDrive - BRGM\Pro\AMORAD\ArticleCarteNationale\GitHub\TestGit\premache\InputsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -750,9 +750,6 @@
     <t>"Code" is the code that should be indicated in the the shapefile.</t>
   </si>
   <si>
-    <t>It is divided in several sheets.</t>
-  </si>
-  <si>
     <t>This spreadsheet is used by the PREMACHE toolbox to create runoff and erosion models inputs. It is based on data from the Bourville catchment as described in the manuscript.</t>
   </si>
   <si>
@@ -880,6 +877,9 @@
   </si>
   <si>
     <t>Values from these tables were defined in Cerdan et al. (2001) and Cerdan et al. (2002)</t>
+  </si>
+  <si>
+    <t>It is divided in several sheets, defining soil surface state initial values, temporal evolutions, and values to convert soil surface state into model inputs</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -2063,25 +2063,25 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2210,8 +2210,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2219,72 +2219,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2329,6 +2263,72 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2654,7 +2654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2668,16 +2670,16 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="139" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2717,7 +2719,7 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="139" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2728,7 +2730,7 @@
     </row>
     <row r="15" spans="1:1" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="161" t="s">
+      <c r="A16" s="139" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2738,7 +2740,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="161" t="s">
+      <c r="A19" s="139" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2754,11 +2756,11 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="161" t="s">
+      <c r="A26" s="139" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3824,7 +3826,7 @@
     <col min="6" max="7" width="30.5703125" style="37" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" style="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="71.140625" style="154" customWidth="1"/>
+    <col min="10" max="10" width="71.140625" style="132" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="37"/>
   </cols>
   <sheetData>
@@ -3856,7 +3858,7 @@
       <c r="I1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="153" t="s">
+      <c r="J1" s="131" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4417,7 +4419,7 @@
         <v>57</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K18" s="33"/>
     </row>
@@ -4516,7 +4518,7 @@
         <v>57</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K21" s="33"/>
     </row>
@@ -4813,7 +4815,7 @@
         <v>58</v>
       </c>
       <c r="J30" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K30" s="33"/>
     </row>
@@ -5242,7 +5244,7 @@
         <v>59</v>
       </c>
       <c r="J43" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K43" s="33"/>
     </row>
@@ -5275,7 +5277,7 @@
         <v>59</v>
       </c>
       <c r="J44" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K44" s="33"/>
     </row>
@@ -5308,7 +5310,7 @@
         <v>59</v>
       </c>
       <c r="J45" s="33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K45" s="33"/>
     </row>
@@ -5341,7 +5343,7 @@
         <v>59</v>
       </c>
       <c r="J46" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K46" s="33"/>
     </row>
@@ -5473,7 +5475,7 @@
         <v>60</v>
       </c>
       <c r="J50" s="33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K50" s="33"/>
     </row>
@@ -5770,7 +5772,7 @@
         <v>61</v>
       </c>
       <c r="J59" s="33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K59" s="33"/>
     </row>
@@ -5803,7 +5805,7 @@
         <v>61</v>
       </c>
       <c r="J60" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K60" s="33"/>
     </row>
@@ -5836,7 +5838,7 @@
         <v>61</v>
       </c>
       <c r="J61" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K61" s="33"/>
     </row>
@@ -5869,7 +5871,7 @@
         <v>61</v>
       </c>
       <c r="J62" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K62" s="33"/>
     </row>
@@ -5902,7 +5904,7 @@
         <v>61</v>
       </c>
       <c r="J63" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K63" s="33"/>
     </row>
@@ -5935,7 +5937,7 @@
         <v>61</v>
       </c>
       <c r="J64" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K64" s="33"/>
     </row>
@@ -5968,7 +5970,7 @@
         <v>61</v>
       </c>
       <c r="J65" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K65" s="33"/>
     </row>
@@ -6001,7 +6003,7 @@
         <v>61</v>
       </c>
       <c r="J66" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K66" s="33"/>
     </row>
@@ -6034,7 +6036,7 @@
         <v>61</v>
       </c>
       <c r="J67" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K67" s="33"/>
     </row>
@@ -6067,7 +6069,7 @@
         <v>61</v>
       </c>
       <c r="J68" s="33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K68" s="33"/>
     </row>
@@ -6100,7 +6102,7 @@
         <v>61</v>
       </c>
       <c r="J69" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K69" s="33"/>
     </row>
@@ -6133,7 +6135,7 @@
         <v>61</v>
       </c>
       <c r="J70" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K70" s="33"/>
     </row>
@@ -6199,7 +6201,7 @@
         <v>61</v>
       </c>
       <c r="J72" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K72" s="33"/>
     </row>
@@ -6232,7 +6234,7 @@
         <v>61</v>
       </c>
       <c r="J73" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K73" s="33"/>
     </row>
@@ -6265,7 +6267,7 @@
         <v>61</v>
       </c>
       <c r="J74" s="33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K74" s="33"/>
     </row>
@@ -6298,7 +6300,7 @@
         <v>61</v>
       </c>
       <c r="J75" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K75" s="33"/>
     </row>
@@ -6331,7 +6333,7 @@
         <v>61</v>
       </c>
       <c r="J76" s="33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K76" s="33"/>
     </row>
@@ -6364,7 +6366,7 @@
         <v>61</v>
       </c>
       <c r="J77" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K77" s="33"/>
     </row>
@@ -6397,7 +6399,7 @@
         <v>61</v>
       </c>
       <c r="J78" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K78" s="33"/>
     </row>
@@ -6430,7 +6432,7 @@
         <v>61</v>
       </c>
       <c r="J79" s="33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K79" s="33"/>
     </row>
@@ -6463,7 +6465,7 @@
         <v>61</v>
       </c>
       <c r="J80" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K80" s="33"/>
     </row>
@@ -6496,7 +6498,7 @@
         <v>61</v>
       </c>
       <c r="J81" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K81" s="33"/>
     </row>
@@ -6529,7 +6531,7 @@
         <v>61</v>
       </c>
       <c r="J82" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K82" s="33"/>
     </row>
@@ -6562,7 +6564,7 @@
         <v>61</v>
       </c>
       <c r="J83" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K83" s="33"/>
     </row>
@@ -6595,7 +6597,7 @@
         <v>61</v>
       </c>
       <c r="J84" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K84" s="33"/>
     </row>
@@ -6628,7 +6630,7 @@
         <v>61</v>
       </c>
       <c r="J85" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K85" s="33"/>
     </row>
@@ -6694,7 +6696,7 @@
         <v>61</v>
       </c>
       <c r="J87" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K87" s="33"/>
     </row>
@@ -6727,7 +6729,7 @@
         <v>61</v>
       </c>
       <c r="J88" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K88" s="33"/>
     </row>
@@ -6793,7 +6795,7 @@
         <v>61</v>
       </c>
       <c r="J90" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K90" s="33"/>
     </row>
@@ -6826,7 +6828,7 @@
         <v>61</v>
       </c>
       <c r="J91" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K91" s="33"/>
     </row>
@@ -6859,7 +6861,7 @@
         <v>61</v>
       </c>
       <c r="J92" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K92" s="33"/>
     </row>
@@ -7321,7 +7323,7 @@
         <v>62</v>
       </c>
       <c r="J106" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K106" s="33"/>
     </row>
@@ -7354,7 +7356,7 @@
         <v>62</v>
       </c>
       <c r="J107" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K107" s="33"/>
     </row>
@@ -7447,9 +7449,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="148"/>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
+      <c r="A1" s="126"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
       <c r="D1" s="39" t="s">
         <v>139</v>
       </c>
@@ -7464,26 +7466,26 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="155"/>
-      <c r="B2" s="156" t="s">
+      <c r="A2" s="133"/>
+      <c r="B2" s="134" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="157" t="s">
+      <c r="C2" s="135" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="158" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="159" t="s">
+      <c r="D2" s="136" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="159" t="s">
+      <c r="G2" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="160" t="s">
+      <c r="H2" s="138" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="119"/>
@@ -7493,7 +7495,7 @@
       <c r="O2" s="120"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="143" t="s">
         <v>132</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -7524,7 +7526,7 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
+      <c r="A4" s="143"/>
       <c r="B4" s="17" t="s">
         <v>74</v>
       </c>
@@ -7543,7 +7545,7 @@
       <c r="G4" s="121">
         <v>114</v>
       </c>
-      <c r="H4" s="150">
+      <c r="H4" s="128">
         <v>124</v>
       </c>
       <c r="K4" s="2"/>
@@ -7553,7 +7555,7 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="128"/>
+      <c r="A5" s="143"/>
       <c r="B5" s="17" t="s">
         <v>126</v>
       </c>
@@ -7582,7 +7584,7 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="128"/>
+      <c r="A6" s="143"/>
       <c r="B6" s="17" t="s">
         <v>127</v>
       </c>
@@ -7611,7 +7613,7 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="128"/>
+      <c r="A7" s="143"/>
       <c r="B7" s="17" t="s">
         <v>78</v>
       </c>
@@ -7640,7 +7642,7 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
+      <c r="A8" s="143"/>
       <c r="B8" s="17" t="s">
         <v>124</v>
       </c>
@@ -7669,7 +7671,7 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="128"/>
+      <c r="A9" s="143"/>
       <c r="B9" s="17" t="s">
         <v>80</v>
       </c>
@@ -7698,7 +7700,7 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="128"/>
+      <c r="A10" s="143"/>
       <c r="B10" s="17" t="s">
         <v>128</v>
       </c>
@@ -7727,7 +7729,7 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="128"/>
+      <c r="A11" s="143"/>
       <c r="B11" s="17" t="s">
         <v>81</v>
       </c>
@@ -7756,7 +7758,7 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="128"/>
+      <c r="A12" s="143"/>
       <c r="B12" s="17" t="s">
         <v>129</v>
       </c>
@@ -7785,7 +7787,7 @@
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="128"/>
+      <c r="A13" s="143"/>
       <c r="B13" s="17" t="s">
         <v>131</v>
       </c>
@@ -7814,7 +7816,7 @@
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="129"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="18" t="s">
         <v>130</v>
       </c>
@@ -7852,7 +7854,7 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="145" t="s">
         <v>133</v>
       </c>
       <c r="B16" s="124" t="s">
@@ -7873,12 +7875,12 @@
       <c r="G16" s="5">
         <v>10</v>
       </c>
-      <c r="H16" s="151" t="s">
+      <c r="H16" s="129" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="131"/>
+      <c r="A17" s="146"/>
       <c r="B17" s="125" t="s">
         <v>137</v>
       </c>
@@ -7897,7 +7899,7 @@
       <c r="G17" s="8">
         <v>15</v>
       </c>
-      <c r="H17" s="152" t="s">
+      <c r="H17" s="130" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7912,7 +7914,7 @@
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="147" t="s">
         <v>134</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -7921,27 +7923,27 @@
       <c r="C19" s="22">
         <v>1</v>
       </c>
-      <c r="D19" s="132" t="s">
+      <c r="D19" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="133"/>
-      <c r="F19" s="133"/>
-      <c r="G19" s="133"/>
-      <c r="H19" s="134"/>
+      <c r="E19" s="150"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="150"/>
+      <c r="H19" s="151"/>
     </row>
     <row r="20" spans="1:8" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="127"/>
+      <c r="A20" s="148"/>
       <c r="B20" s="21" t="s">
         <v>137</v>
       </c>
       <c r="C20" s="23">
         <v>2</v>
       </c>
-      <c r="D20" s="135"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="136"/>
-      <c r="H20" s="137"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="153"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="153"/>
+      <c r="H20" s="154"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
@@ -8040,13 +8042,13 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="66"/>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="155" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="140"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="157"/>
       <c r="G1" s="71"/>
       <c r="H1" s="71"/>
       <c r="I1" s="71"/>
@@ -8300,13 +8302,13 @@
       <c r="A1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="140"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="157"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
@@ -8628,26 +8630,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="143"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="160"/>
     </row>
     <row r="2" spans="1:7" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="163" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="145"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="161"/>
+      <c r="F2" s="162"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -9008,12 +9010,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="143"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="160"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="116" t="s">
@@ -9125,15 +9127,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="158" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="143"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="160"/>
       <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -10261,13 +10263,13 @@
       <c r="L46" s="37"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="162" t="s">
+      <c r="A47" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="163" t="s">
+      <c r="B47" s="141" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="164" t="s">
+      <c r="C47" s="142" t="s">
         <v>45</v>
       </c>
       <c r="D47" s="97">
@@ -10571,22 +10573,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="143"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="160"/>
     </row>
     <row r="2" spans="1:5" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="112"/>
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="164" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="145"/>
+      <c r="C2" s="161"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="162"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="112" t="s">
@@ -10822,6 +10824,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090E2F3373884014A91EB531DC859069F" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="68bb6f05d204b4f7a11ff7c2fc734609">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="546f304f191a714413a456dcee5e7784" ns2:_="">
     <xsd:import namespace="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8"/>
@@ -10953,22 +10970,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD9BEAA6-C677-4677-A34B-6D33B61C7671}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72962638-AE51-415A-89B8-945EEA70B9EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36485FDE-3765-4334-96EA-B947DBAEB3EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10984,28 +11010,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72962638-AE51-415A-89B8-945EEA70B9EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD9BEAA6-C677-4677-A34B-6D33B61C7671}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
deplacement pram.yma dans inputdat
</commit_message>
<xml_diff>
--- a/InputsData/Data&Values.xlsx
+++ b/InputsData/Data&Values.xlsx
@@ -10839,8 +10839,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090E2F3373884014A91EB531DC859069F" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="68bb6f05d204b4f7a11ff7c2fc734609">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="546f304f191a714413a456dcee5e7784" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090E2F3373884014A91EB531DC859069F" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="09426021cb9970de231e32d57c566f52">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ee9576dbc2b49a0a47f52fea154cdf9" ns2:_="">
     <xsd:import namespace="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -10850,6 +10850,12 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -10868,6 +10874,40 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -10995,19 +11035,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36485FDE-3765-4334-96EA-B947DBAEB3EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ea60a7b2-88aa-41e2-9676-c02d4cc6f5e8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFBB82F-CC5F-47C0-A3CE-6B0B3CDF0264}"/>
 </file>
</xml_diff>